<commit_message>
added accuracy check function to training
</commit_message>
<xml_diff>
--- a/results/sift_bins_test.xlsx
+++ b/results/sift_bins_test.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torifujinami/Documents/stanford/spring2018/cs231n/project/CS231n-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torifujinami/Documents/stanford/spring2018/cs231n/project/CS231n-Project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729381E7-3676-B04F-B367-9D3515B9E8C1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404E8F46-507D-1A44-855A-8BA5AE2D6AFB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sift_bins_test" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">sift_bins_test!$B$1:$B$40</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">sift_bins_test!$E$1:$E$40</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">sift_bins_test!$G:$G</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
@@ -1132,6 +1137,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SIFT Feature Distances</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1171,6 +1201,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>matching</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1388,6 +1421,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>non-matching</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -1638,7 +1674,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1658,33 +1694,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="85052047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -3235,7 +3244,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E7" zoomScale="133" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3292,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G2:G40" si="0">A3-6</f>
+        <f t="shared" ref="G3:G39" si="0">A3-6</f>
         <v>25</v>
       </c>
     </row>

</xml_diff>